<commit_message>
Se agrego campo Manifiestos y Configuracion basic
</commit_message>
<xml_diff>
--- a/ArchivosExcel/relaciones.xlsx
+++ b/ArchivosExcel/relaciones.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/904702f6d0479124/Desktop/CODIGO ESTADIAS/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/904702f6d0479124/Documentos/Sistema Integral de Gestión Liverpool/ArchivosExcel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:1_{C922AA6B-3151-46B1-B8FE-1919D214F2BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FAADFE83-B3FA-48B0-B6E4-1818BDAF48DC}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="13_ncr:1_{C922AA6B-3151-46B1-B8FE-1919D214F2BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{150F4CFF-AF4B-40BB-8979-68E4886B2488}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{B5FFFD52-C1CF-4748-BBE8-8FA2D60D5EDD}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B5FFFD52-C1CF-4748-BBE8-8FA2D60D5EDD}"/>
   </bookViews>
   <sheets>
     <sheet name="Usuarios" sheetId="1" r:id="rId1"/>
@@ -20,15 +20,6 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -126,7 +117,7 @@
     <t>Yuviana</t>
   </si>
   <si>
-    <t>ygtiripitig@liverpool.com</t>
+    <t>ygtiripitig@liverpool.com.mx</t>
   </si>
 </sst>
 </file>
@@ -522,8 +513,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58494B71-9843-4C04-979A-50D0244DB90B}">
   <dimension ref="A1:F147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A126" workbookViewId="0">
-      <selection activeCell="A133" sqref="A133:A147"/>
+    <sheetView tabSelected="1" topLeftCell="A123" workbookViewId="0">
+      <selection activeCell="G146" sqref="G146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2597,6 +2588,8 @@
     <hyperlink ref="A3" r:id="rId1" xr:uid="{B3993411-8498-429D-A808-678F8386BE9A}"/>
     <hyperlink ref="A2" r:id="rId2" xr:uid="{0B461813-A3E4-4D2B-BB70-BF2BFB06CC2F}"/>
     <hyperlink ref="A4:A24" r:id="rId3" display="figaspars@liverpool.com.mx" xr:uid="{C89E0445-341B-4FF6-B559-FE20666192A7}"/>
+    <hyperlink ref="A133" r:id="rId4" xr:uid="{7B8E99CB-8565-4A45-A167-DD2B5067D3E1}"/>
+    <hyperlink ref="A134:A147" r:id="rId5" display="ygtiripitig@liverpool.com.mx" xr:uid="{8B28E55D-00B8-402A-ADF1-369C6B96D57F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>